<commit_message>
Child exemptions increase for 2024
</commit_message>
<xml_diff>
--- a/Federal/f1040s8-2023.xlsx
+++ b/Federal/f1040s8-2023.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="IRS f1040 8812" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -174,9 +174,6 @@
     <t>16b</t>
   </si>
   <si>
-    <t>Number of qualifying children under 17 with the required social security number x $1,500:</t>
-  </si>
-  <si>
     <t>TIP: The number of children you use for this line is the same as the number of children you used for line 4.</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
   </si>
   <si>
     <t>Multiply the amount on line 19 by 15% (0.15) and enter the result</t>
-  </si>
-  <si>
-    <t>Next. On line 16b, is the amount $4,500 or more?</t>
   </si>
   <si>
     <t>No: If you are a bona fide resident of Puerto Rico, go to line 21. Otherwise, skip Part II-B and enter the smaller of line 17 or line 20 on line 27.</t>
@@ -304,6 +298,12 @@
   </si>
   <si>
     <t xml:space="preserve">No. STOP. You cannot take the child tax credit, credit for other dependents, or additional child tax credit. Skip Parts II-A and II-B.  Enter -0- on lines 14 and 27. </t>
+  </si>
+  <si>
+    <t>Number of qualifying children under 17 with the required social security number x $1,700:</t>
+  </si>
+  <si>
+    <t>Next. On line 16b, is the amount $5,100 or more?</t>
   </si>
 </sst>
 </file>
@@ -1084,6 +1084,61 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1096,62 +1151,7 @@
     <xf numFmtId="0" fontId="22" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1476,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1489,86 +1489,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="41"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1578,13 +1578,13 @@
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
       <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1596,13 +1596,13 @@
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1614,13 +1614,13 @@
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1632,15 +1632,15 @@
       <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1653,15 +1653,15 @@
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1674,13 +1674,13 @@
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1692,15 +1692,15 @@
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1731,15 +1731,15 @@
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1752,15 +1752,15 @@
       <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
       <c r="I16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1773,15 +1773,15 @@
       <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
       <c r="I17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1791,15 +1791,15 @@
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1812,15 +1812,15 @@
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1830,46 +1830,46 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="45"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="52"/>
+      <c r="A21" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="40"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1882,15 +1882,15 @@
       <c r="A23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
       <c r="I23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1900,15 +1900,15 @@
       <c r="A24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
       <c r="I24" s="1" t="s">
         <v>38</v>
       </c>
@@ -1918,101 +1918,101 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="45"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="37"/>
     </row>
     <row r="26" spans="1:10" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="43"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
     </row>
     <row r="29" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="41"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="28"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="47"/>
     </row>
     <row r="33" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
@@ -2058,7 +2058,7 @@
         <v>50</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
@@ -2068,32 +2068,32 @@
         <v>50</v>
       </c>
       <c r="H35" s="19">
-        <f>1500*H12</f>
+        <f>1700*H12</f>
         <v>0</v>
       </c>
       <c r="I35" s="20"/>
       <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="36"/>
+      <c r="A36" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="47"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>53</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>54</v>
       </c>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
@@ -2102,7 +2102,7 @@
       <c r="G37" s="33"/>
       <c r="H37" s="33"/>
       <c r="I37" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J37" s="18">
         <f>MIN(J34,H35)</f>
@@ -2111,17 +2111,17 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="33" t="s">
         <v>55</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>56</v>
       </c>
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="33"/>
       <c r="G38" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H38" s="19"/>
       <c r="I38" s="20"/>
@@ -2129,63 +2129,63 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="33" t="s">
         <v>57</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>58</v>
       </c>
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="33"/>
       <c r="G39" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H39" s="19"/>
       <c r="I39" s="20"/>
       <c r="J39" s="21"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="47"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="36"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="36"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="47"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" s="37" t="s">
-        <v>87</v>
+        <v>60</v>
+      </c>
+      <c r="B42" s="48" t="s">
+        <v>85</v>
       </c>
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="33"/>
       <c r="G42" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H42" s="19">
         <f>MAX(H38-2500,0)</f>
@@ -2196,10 +2196,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="33" t="s">
         <v>62</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>63</v>
       </c>
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
@@ -2208,7 +2208,7 @@
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
       <c r="I43" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J43" s="18">
         <f>ROUND(0.15*H42,2)</f>
@@ -2216,46 +2216,46 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="47"/>
+    </row>
+    <row r="45" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="47"/>
+    </row>
+    <row r="46" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="36"/>
-    </row>
-    <row r="45" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="36"/>
-    </row>
-    <row r="46" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="24"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="51"/>
     </row>
     <row r="47" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -2263,39 +2263,39 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="27"/>
+      <c r="A48" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="54"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
-      <c r="J49" s="30"/>
+      <c r="A49" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="31"/>
     </row>
     <row r="50" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
@@ -2304,16 +2304,16 @@
       <c r="G50" s="33"/>
       <c r="H50" s="33"/>
       <c r="I50" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J50" s="18"/>
     </row>
     <row r="51" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
@@ -2322,16 +2322,16 @@
       <c r="G51" s="33"/>
       <c r="H51" s="33"/>
       <c r="I51" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J51" s="18"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B52" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
@@ -2340,7 +2340,7 @@
       <c r="G52" s="33"/>
       <c r="H52" s="33"/>
       <c r="I52" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J52" s="18">
         <f>J51+J50</f>
@@ -2348,36 +2348,36 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="36"/>
+      <c r="A53" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="47"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="36"/>
+      <c r="A54" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="47"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B55" s="33" t="s">
         <v>2</v>
@@ -2387,7 +2387,7 @@
       <c r="E55" s="33"/>
       <c r="F55" s="33"/>
       <c r="G55" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H55" s="19"/>
       <c r="I55" s="20"/>
@@ -2395,10 +2395,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B56" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
@@ -2407,7 +2407,7 @@
       <c r="G56" s="33"/>
       <c r="H56" s="33"/>
       <c r="I56" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J56" s="18">
         <f>MAX(J52-H55,0)</f>
@@ -2416,10 +2416,10 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C57" s="33"/>
       <c r="D57" s="33"/>
@@ -2428,7 +2428,7 @@
       <c r="G57" s="33"/>
       <c r="H57" s="33"/>
       <c r="I57" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J57" s="18">
         <f>MAX(J43,J56)</f>
@@ -2436,18 +2436,18 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" s="23"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="24"/>
+      <c r="A58" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="51"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2460,48 +2460,48 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="27"/>
+      <c r="A61" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="53"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="54"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B62" s="29"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="29"/>
-      <c r="I62" s="29"/>
-      <c r="J62" s="30"/>
+      <c r="A62" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="30"/>
+      <c r="J62" s="31"/>
     </row>
     <row r="63" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="31"/>
+        <v>83</v>
+      </c>
+      <c r="B63" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="55"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="55"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="55"/>
       <c r="I63" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J63" s="10">
         <f>MAX(J37,J57)</f>
@@ -2509,29 +2509,57 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="32"/>
-      <c r="H64" s="32"/>
-      <c r="I64" s="32"/>
-      <c r="J64" s="32"/>
+      <c r="A64" s="25"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="A58:J58"/>
+    <mergeCell ref="A61:J61"/>
+    <mergeCell ref="A62:J62"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="A64:J64"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="A53:J53"/>
+    <mergeCell ref="A54:J54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A44:J44"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A32:J32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A27:J27"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="B12:F12"/>
@@ -2544,44 +2572,16 @@
     <mergeCell ref="B19:H19"/>
     <mergeCell ref="A20:J20"/>
     <mergeCell ref="A21:J21"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A32:J32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="A44:J44"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="A45:J45"/>
-    <mergeCell ref="A46:J46"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="A53:J53"/>
-    <mergeCell ref="A54:J54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="A58:J58"/>
-    <mergeCell ref="A61:J61"/>
-    <mergeCell ref="A62:J62"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="A64:J64"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Restore 2023 Schedule 88812 and create 2024 Schedule 88812
I accidentally edited the old one instead of copying it to the current year.
</commit_message>
<xml_diff>
--- a/Federal/f1040s8-2023.xlsx
+++ b/Federal/f1040s8-2023.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="IRS f1040 8812" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -174,6 +174,9 @@
     <t>16b</t>
   </si>
   <si>
+    <t>Number of qualifying children under 17 with the required social security number x $1,500:</t>
+  </si>
+  <si>
     <t>TIP: The number of children you use for this line is the same as the number of children you used for line 4.</t>
   </si>
   <si>
@@ -208,6 +211,9 @@
   </si>
   <si>
     <t>Multiply the amount on line 19 by 15% (0.15) and enter the result</t>
+  </si>
+  <si>
+    <t>Next. On line 16b, is the amount $4,500 or more?</t>
   </si>
   <si>
     <t>No: If you are a bona fide resident of Puerto Rico, go to line 21. Otherwise, skip Part II-B and enter the smaller of line 17 or line 20 on line 27.</t>
@@ -298,12 +304,6 @@
   </si>
   <si>
     <t xml:space="preserve">No. STOP. You cannot take the child tax credit, credit for other dependents, or additional child tax credit. Skip Parts II-A and II-B.  Enter -0- on lines 14 and 27. </t>
-  </si>
-  <si>
-    <t>Number of qualifying children under 17 with the required social security number x $1,700:</t>
-  </si>
-  <si>
-    <t>Next. On line 16b, is the amount $5,100 or more?</t>
   </si>
 </sst>
 </file>
@@ -1084,30 +1084,58 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1117,41 +1145,13 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1476,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1489,86 +1489,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="31"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1578,13 +1578,13 @@
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1596,13 +1596,13 @@
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1614,13 +1614,13 @@
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1632,15 +1632,15 @@
       <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1653,15 +1653,15 @@
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1674,13 +1674,13 @@
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1692,15 +1692,15 @@
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
       <c r="I13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1731,15 +1731,15 @@
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1752,15 +1752,15 @@
       <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
       <c r="I16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1773,15 +1773,15 @@
       <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
       <c r="I17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1791,15 +1791,15 @@
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
       <c r="I18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1812,15 +1812,15 @@
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
       <c r="I19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1830,46 +1830,46 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="37"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="40"/>
+      <c r="A21" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="52"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
       <c r="I22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1882,15 +1882,15 @@
       <c r="A23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
       <c r="I23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1900,15 +1900,15 @@
       <c r="A24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
       <c r="I24" s="1" t="s">
         <v>38</v>
       </c>
@@ -1918,101 +1918,101 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="37"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="45"/>
     </row>
     <row r="26" spans="1:10" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="43"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="48"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="28"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="41"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="47"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="36"/>
     </row>
     <row r="33" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
@@ -2058,7 +2058,7 @@
         <v>50</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
@@ -2068,32 +2068,32 @@
         <v>50</v>
       </c>
       <c r="H35" s="19">
-        <f>1700*H12</f>
+        <f>1500*H12</f>
         <v>0</v>
       </c>
       <c r="I35" s="20"/>
       <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="46"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="47"/>
+      <c r="A36" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="36"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
@@ -2102,7 +2102,7 @@
       <c r="G37" s="33"/>
       <c r="H37" s="33"/>
       <c r="I37" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J37" s="18">
         <f>MIN(J34,H35)</f>
@@ -2111,17 +2111,17 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="33"/>
       <c r="G38" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H38" s="19"/>
       <c r="I38" s="20"/>
@@ -2129,63 +2129,63 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="33"/>
       <c r="G39" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H39" s="19"/>
       <c r="I39" s="20"/>
       <c r="J39" s="21"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="47"/>
+      <c r="A40" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="36"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="47"/>
+      <c r="A41" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="36"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="48" t="s">
-        <v>85</v>
+        <v>61</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>87</v>
       </c>
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="33"/>
       <c r="G42" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H42" s="19">
         <f>MAX(H38-2500,0)</f>
@@ -2196,10 +2196,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
@@ -2208,7 +2208,7 @@
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
       <c r="I43" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J43" s="18">
         <f>ROUND(0.15*H42,2)</f>
@@ -2216,46 +2216,46 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="46"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="47"/>
+      <c r="A44" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="47"/>
+      <c r="A45" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="51"/>
+      <c r="A46" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="24"/>
     </row>
     <row r="47" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -2263,39 +2263,39 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="54"/>
+      <c r="A48" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="27"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="31"/>
+      <c r="A49" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="30"/>
     </row>
     <row r="50" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
@@ -2304,16 +2304,16 @@
       <c r="G50" s="33"/>
       <c r="H50" s="33"/>
       <c r="I50" s="17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J50" s="18"/>
     </row>
     <row r="51" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
@@ -2322,16 +2322,16 @@
       <c r="G51" s="33"/>
       <c r="H51" s="33"/>
       <c r="I51" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J51" s="18"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B52" s="33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
@@ -2340,7 +2340,7 @@
       <c r="G52" s="33"/>
       <c r="H52" s="33"/>
       <c r="I52" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J52" s="18">
         <f>J51+J50</f>
@@ -2348,36 +2348,36 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="46"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="47"/>
+      <c r="A53" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="36"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B54" s="46"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="46"/>
-      <c r="H54" s="46"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="47"/>
+      <c r="A54" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="36"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B55" s="33" t="s">
         <v>2</v>
@@ -2387,7 +2387,7 @@
       <c r="E55" s="33"/>
       <c r="F55" s="33"/>
       <c r="G55" s="17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H55" s="19"/>
       <c r="I55" s="20"/>
@@ -2395,10 +2395,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B56" s="33" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
@@ -2407,7 +2407,7 @@
       <c r="G56" s="33"/>
       <c r="H56" s="33"/>
       <c r="I56" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J56" s="18">
         <f>MAX(J52-H55,0)</f>
@@ -2416,10 +2416,10 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C57" s="33"/>
       <c r="D57" s="33"/>
@@ -2428,7 +2428,7 @@
       <c r="G57" s="33"/>
       <c r="H57" s="33"/>
       <c r="I57" s="17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J57" s="18">
         <f>MAX(J43,J56)</f>
@@ -2436,18 +2436,18 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="50"/>
-      <c r="H58" s="50"/>
-      <c r="I58" s="50"/>
-      <c r="J58" s="51"/>
+      <c r="A58" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="24"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2460,48 +2460,48 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" s="53"/>
-      <c r="C61" s="53"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="53"/>
-      <c r="G61" s="53"/>
-      <c r="H61" s="53"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="54"/>
+      <c r="A61" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="27"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="31"/>
+      <c r="A62" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="30"/>
     </row>
     <row r="63" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B63" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="C63" s="55"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="55"/>
-      <c r="H63" s="55"/>
+        <v>85</v>
+      </c>
+      <c r="B63" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
       <c r="I63" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J63" s="10">
         <f>MAX(J37,J57)</f>
@@ -2509,24 +2509,62 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="25"/>
-      <c r="J64" s="25"/>
+      <c r="A64" s="32"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A58:J58"/>
-    <mergeCell ref="A61:J61"/>
-    <mergeCell ref="A62:J62"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="A64:J64"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A32:J32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A44:J44"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="A45:J45"/>
     <mergeCell ref="A46:J46"/>
@@ -2539,49 +2577,11 @@
     <mergeCell ref="A54:J54"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="B56:H56"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="A44:J44"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A32:J32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="A58:J58"/>
+    <mergeCell ref="A61:J61"/>
+    <mergeCell ref="A62:J62"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="A64:J64"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>